<commit_message>
Add suggestions to quotation unit codes and item names
</commit_message>
<xml_diff>
--- a/public/reference/toolist.xlsx
+++ b/public/reference/toolist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kameredavid\Desktop\Projects\opensource\kanschedule\public\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8D1D6E-83E0-4A38-AC64-8AAE99065C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DFC116-3643-4A59-AA34-5438DA0530CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{49A8AD54-475A-47BE-A1FA-50AB35883E38}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="482">
   <si>
     <t>Current Pricing</t>
   </si>
@@ -1468,6 +1468,9 @@
   </si>
   <si>
     <t>Time Needed</t>
+  </si>
+  <si>
+    <t>Product Name</t>
   </si>
 </sst>
 </file>
@@ -1996,9 +1999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23682914-449E-4FF9-828C-D87A9F617CD7}">
   <dimension ref="A1:M235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2015,7 +2016,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
+      <c r="A1" s="16" t="s">
+        <v>481</v>
+      </c>
       <c r="B1">
         <f>COUNTIF(C2:C151, "?*")</f>
         <v>0</v>
@@ -2763,7 +2766,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2803,7 +2806,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2843,7 +2846,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -2883,7 +2886,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2916,7 +2919,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>56</v>
       </c>
@@ -2954,7 +2957,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -2991,7 +2994,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -3028,7 +3031,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -3065,7 +3068,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -3102,7 +3105,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -3135,7 +3138,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>68</v>
       </c>
@@ -3175,7 +3178,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>70</v>
       </c>
@@ -3215,7 +3218,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -3372,7 +3375,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -3407,7 +3410,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -3439,7 +3442,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -3471,7 +3474,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -3503,7 +3506,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -3535,7 +3538,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -3570,7 +3573,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -3605,7 +3608,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>94</v>
       </c>
@@ -3638,7 +3641,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -3670,7 +3673,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>98</v>
       </c>
@@ -3702,7 +3705,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -3734,7 +3737,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>102</v>
       </c>
@@ -3766,7 +3769,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -3798,7 +3801,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>106</v>
       </c>
@@ -3830,7 +3833,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -3862,7 +3865,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -3902,7 +3905,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -3942,7 +3945,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -3979,7 +3982,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>117</v>
       </c>
@@ -4016,7 +4019,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -4053,7 +4056,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -4088,7 +4091,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>123</v>
       </c>
@@ -4123,7 +4126,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>125</v>
       </c>
@@ -4158,7 +4161,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -4193,7 +4196,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>129</v>
       </c>
@@ -4228,7 +4231,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -4263,7 +4266,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>133</v>
       </c>
@@ -4303,7 +4306,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>135</v>
       </c>
@@ -4343,7 +4346,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>137</v>
       </c>
@@ -4383,7 +4386,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>139</v>
       </c>
@@ -4423,7 +4426,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>141</v>
       </c>
@@ -4460,7 +4463,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>143</v>
       </c>
@@ -4497,7 +4500,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>145</v>
       </c>
@@ -4534,7 +4537,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>147</v>
       </c>
@@ -4576,7 +4579,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -4613,7 +4616,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>151</v>
       </c>
@@ -4650,7 +4653,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>153</v>
       </c>
@@ -4687,7 +4690,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>155</v>
       </c>
@@ -4724,7 +4727,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>157</v>
       </c>
@@ -4761,7 +4764,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="16" t="s">
         <v>159</v>
       </c>
@@ -4799,7 +4802,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16" t="s">
         <v>161</v>
       </c>
@@ -4836,7 +4839,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>163</v>
       </c>
@@ -4878,7 +4881,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16" t="s">
         <v>165</v>
       </c>
@@ -4918,7 +4921,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>167</v>
       </c>
@@ -4955,7 +4958,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>169</v>
       </c>
@@ -4995,7 +4998,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>171</v>
       </c>
@@ -5034,7 +5037,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -5071,7 +5074,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>175</v>
       </c>
@@ -5111,7 +5114,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>177</v>
       </c>
@@ -5151,7 +5154,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>179</v>
       </c>
@@ -5188,7 +5191,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>181</v>
       </c>
@@ -5220,7 +5223,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>183</v>
       </c>
@@ -5252,7 +5255,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>185</v>
       </c>
@@ -5289,7 +5292,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>187</v>
       </c>
@@ -5326,7 +5329,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>189</v>
       </c>
@@ -5358,7 +5361,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>191</v>
       </c>
@@ -5395,7 +5398,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>193</v>
       </c>
@@ -5430,7 +5433,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>195</v>
       </c>
@@ -5467,7 +5470,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>197</v>
       </c>
@@ -5505,7 +5508,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>199</v>
       </c>
@@ -5543,7 +5546,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>201</v>
       </c>
@@ -5580,7 +5583,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>203</v>
       </c>
@@ -5617,7 +5620,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>205</v>
       </c>
@@ -5655,7 +5658,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>207</v>
       </c>
@@ -5693,7 +5696,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>209</v>
       </c>
@@ -5731,7 +5734,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>211</v>
       </c>
@@ -5769,7 +5772,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>213</v>
       </c>
@@ -5807,7 +5810,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>215</v>
       </c>
@@ -5845,7 +5848,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>217</v>
       </c>
@@ -5883,7 +5886,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>219</v>
       </c>
@@ -5921,7 +5924,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>221</v>
       </c>
@@ -5959,7 +5962,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>223</v>
       </c>
@@ -5997,7 +6000,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>225</v>
       </c>
@@ -6034,7 +6037,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>229</v>
       </c>
@@ -6071,7 +6074,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>231</v>
       </c>
@@ -6109,7 +6112,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>233</v>
       </c>
@@ -6147,7 +6150,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>235</v>
       </c>
@@ -6185,7 +6188,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>237</v>
       </c>
@@ -6223,7 +6226,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>239</v>
       </c>
@@ -6261,7 +6264,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>241</v>
       </c>
@@ -6299,7 +6302,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>243</v>
       </c>
@@ -6337,7 +6340,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>245</v>
       </c>
@@ -6375,7 +6378,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>247</v>
       </c>
@@ -6412,7 +6415,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>249</v>
       </c>
@@ -6449,7 +6452,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>251</v>
       </c>
@@ -6524,7 +6527,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>255</v>
       </c>
@@ -6550,7 +6553,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="16" t="s">
         <v>257</v>
       </c>
@@ -6588,7 +6591,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>259</v>
       </c>
@@ -6623,7 +6626,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>261</v>
       </c>
@@ -6658,7 +6661,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>263</v>
       </c>
@@ -6693,7 +6696,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>266</v>
       </c>
@@ -6733,7 +6736,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>268</v>
       </c>
@@ -6773,7 +6776,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>270</v>
       </c>
@@ -6813,7 +6816,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>272</v>
       </c>
@@ -6853,7 +6856,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>274</v>
       </c>
@@ -6890,7 +6893,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="16" t="s">
         <v>276</v>
       </c>
@@ -6928,7 +6931,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="16" t="s">
         <v>278</v>
       </c>
@@ -7036,7 +7039,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>284</v>
       </c>
@@ -7268,7 +7271,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="16" t="s">
         <v>296</v>
       </c>
@@ -7344,7 +7347,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="24" t="s">
         <v>301</v>
       </c>
@@ -7381,7 +7384,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="24" t="s">
         <v>303</v>
       </c>
@@ -7531,7 +7534,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="27" t="s">
         <v>311</v>
       </c>
@@ -7568,7 +7571,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="24" t="s">
         <v>313</v>
       </c>
@@ -7605,7 +7608,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="24" t="s">
         <v>315</v>
       </c>
@@ -7642,7 +7645,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="27" t="s">
         <v>317</v>
       </c>
@@ -7716,7 +7719,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="27" t="s">
         <v>321</v>
       </c>
@@ -7754,7 +7757,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="24" t="s">
         <v>323</v>
       </c>
@@ -7794,7 +7797,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="24" t="s">
         <v>325</v>
       </c>
@@ -7831,7 +7834,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="27" t="s">
         <v>327</v>
       </c>
@@ -7869,7 +7872,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="159" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="27" t="s">
         <v>329</v>
       </c>
@@ -7909,7 +7912,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="160" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="24" t="s">
         <v>331</v>
       </c>
@@ -7949,7 +7952,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="161" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="24" t="s">
         <v>333</v>
       </c>
@@ -7986,7 +7989,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="24" t="s">
         <v>335</v>
       </c>
@@ -8024,7 +8027,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="163" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="27" t="s">
         <v>337</v>
       </c>
@@ -8062,7 +8065,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="164" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="24" t="s">
         <v>339</v>
       </c>
@@ -8099,7 +8102,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="165" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>341</v>
       </c>
@@ -8136,7 +8139,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="166" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="24" t="s">
         <v>343</v>
       </c>
@@ -8173,7 +8176,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="167" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>345</v>
       </c>
@@ -9615,7 +9618,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="217" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>444</v>
       </c>
@@ -9653,7 +9656,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="218" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>446</v>
       </c>
@@ -9691,7 +9694,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="219" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>448</v>
       </c>
@@ -9729,7 +9732,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>450</v>
       </c>
@@ -9767,7 +9770,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="221" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>452</v>
       </c>
@@ -9939,7 +9942,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="227" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="24" t="s">
         <v>464</v>
       </c>
@@ -9977,7 +9980,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="228" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>466</v>
       </c>
@@ -10054,7 +10057,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="230" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>470</v>
       </c>
@@ -10094,7 +10097,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="231" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>471</v>
       </c>
@@ -10129,7 +10132,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="232" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>472</v>
       </c>
@@ -10163,7 +10166,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>473</v>
       </c>
@@ -10195,7 +10198,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="234" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>475</v>
       </c>
@@ -10227,7 +10230,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="235" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>477</v>
       </c>
@@ -10265,5 +10268,6 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Calibrated Gas " prompt="Calibrated gas is expendable after 1 year._x000a_1 Year value at $100.00 _x000a_Depreciation Value set for 5 years @ 261 days per year. " sqref="J83" xr:uid="{9AE48071-0F3E-4C85-98C6-9A6366ADEB26}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>